<commit_message>
Updated Tablica.xls and latex folder.
</commit_message>
<xml_diff>
--- a/excel/Tablica.xlsx
+++ b/excel/Tablica.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13880" tabRatio="500"/>
+    <workbookView xWindow="30260" yWindow="-3100" windowWidth="27320" windowHeight="13500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>simple</t>
   </si>
@@ -45,9 +45,6 @@
     <t>probabilistic</t>
   </si>
   <si>
-    <t>crypto</t>
-  </si>
-  <si>
     <t>mux 11</t>
   </si>
   <si>
@@ -97,6 +94,15 @@
   </si>
   <si>
     <t>semantic/simple 1/9</t>
+  </si>
+  <si>
+    <t>crypto 1</t>
+  </si>
+  <si>
+    <t>crypto 4</t>
+  </si>
+  <si>
+    <t>iprojekt</t>
   </si>
 </sst>
 </file>
@@ -126,13 +132,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
@@ -153,6 +152,14 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -164,11 +171,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -200,6 +202,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -225,51 +232,68 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="11" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="17" applyFill="1"/>
+    <xf numFmtId="11" fontId="6" fillId="8" borderId="0" xfId="17" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="14">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+  <cellStyles count="22">
+    <cellStyle name="Explanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="3" builtinId="10"/>
+    <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -598,880 +622,1033 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
-    <col min="7" max="7" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="C1" s="10" t="s">
+    <row r="1" spans="1:13">
+      <c r="B1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="B2" s="8" t="s">
+      <c r="M1" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="B2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="L2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="M2" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="C3">
+      <c r="D3">
+        <v>3.9</v>
+      </c>
+      <c r="E3">
+        <v>427.33333299999998</v>
+      </c>
+      <c r="F3">
+        <v>1.1640448000000001</v>
+      </c>
+      <c r="G3">
+        <v>0.63482333000000002</v>
+      </c>
+      <c r="H3" s="1">
+        <v>5.8471999999999996E-16</v>
+      </c>
+      <c r="I3" s="3">
+        <v>2.4171406700000002</v>
+      </c>
+      <c r="J3" s="3">
         <v>0</v>
       </c>
-      <c r="E3">
-        <v>1.1640448000000001</v>
-      </c>
-      <c r="F3">
-        <v>0.63482333000000002</v>
-      </c>
-      <c r="G3" s="1">
-        <v>5.8471999999999996E-16</v>
-      </c>
-      <c r="H3">
-        <v>2.4171406700000002</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
+      <c r="K3">
         <v>30.747219999999999</v>
       </c>
-      <c r="K3">
+      <c r="L3" s="3">
         <v>70.3</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="M3">
+        <v>16.364896699999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="C4">
-        <v>0</v>
+      <c r="D4">
+        <v>5.3666660000000004</v>
       </c>
       <c r="E4">
+        <v>486.96666670000002</v>
+      </c>
+      <c r="F4">
         <v>1.51229653</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>6.4212023299999998</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>7.2535000000000004E-16</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>5.0484646700000004</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.45233553999999998</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>85.108540000000005</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>59.4</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="M4">
+        <v>16.288783299999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="C5">
-        <v>0.13333329999999999</v>
+      <c r="B5">
+        <v>111</v>
+      </c>
+      <c r="D5">
+        <v>4.8333329999999997</v>
       </c>
       <c r="E5">
+        <v>461.7</v>
+      </c>
+      <c r="F5">
         <v>1.24346859</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>3.9196123300000001</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="4">
         <v>7.5125000000000003E-16</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>4.1872176699999999</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.4976853</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>62.800496699999997</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <v>61.8</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="M5">
+        <v>16.171403300000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="C6">
-        <v>0</v>
+      <c r="D6">
+        <v>4.5999999999999996</v>
       </c>
       <c r="E6">
+        <v>431.76666667000001</v>
+      </c>
+      <c r="F6">
         <v>1.2003219300000001</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>2.0041653300000002</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>6.9204E-16</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>4.6585486700000001</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0.18735260000000001</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>27.226749300000002</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>66.400000000000006</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="M6">
+        <v>16.221446700000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="E7">
+      <c r="D7">
+        <v>4.2</v>
+      </c>
+      <c r="F7">
         <v>1.6424551000000001</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>5.2279523299999999</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>9.835E-4</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>6.5434099999999997</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>0.82343434000000004</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>51.458713299999999</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>61.4</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="M7">
+        <v>16.312249999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="C8">
-        <v>0</v>
+      <c r="D8">
+        <v>4.3</v>
       </c>
       <c r="E8">
+        <v>476.53333300000003</v>
+      </c>
+      <c r="F8">
         <v>1.6177794700000001</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>3.8770926700000001</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>6.5872999999999996E-16</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>5.1089936700000003</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>0.13171603000000001</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>59.151755000000001</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>62.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="M8">
+        <v>16.222923300000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="C9">
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11">
         <v>0.26666659999999998</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="11"/>
+      <c r="F9">
         <v>2.0514364700000001</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>3.8771770000000001</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>5.0608299999999997E-3</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>5.0862743300000002</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>0.16171174999999999</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>46.658380000000001</v>
       </c>
-      <c r="K9" s="1">
+      <c r="L9" s="12">
         <v>58.8</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="M9" s="11"/>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="C10">
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11">
         <v>12.3</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="11"/>
+      <c r="F10">
         <v>18.969425699999999</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>10.622653</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>2.1152359999999999</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>12.636146699999999</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>6.6285039299999999</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>1078.7464299999999</v>
       </c>
-      <c r="K10">
+      <c r="L10" s="11">
         <v>31.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="M10" s="11"/>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="E11" s="9">
+        <v>24</v>
+      </c>
+      <c r="D11">
+        <v>13.966666</v>
+      </c>
+      <c r="F11" s="8">
         <v>0.15859317000000001</v>
       </c>
-      <c r="F11">
+      <c r="G11" s="3">
         <v>0.35</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>0.43794266999999998</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>3.0113536700000001</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>0.13773753</v>
       </c>
-      <c r="J11">
+      <c r="K11" s="3">
         <v>15.9178143</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>19</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>20</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>21</v>
       </c>
-      <c r="E20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21" s="1">
-        <v>0</v>
+        <v>16.5474</v>
       </c>
       <c r="C21" s="1">
-        <v>85</v>
+        <v>10774.9</v>
       </c>
       <c r="D21" s="1">
-        <v>0</v>
-      </c>
-      <c r="E21" s="2">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>16.5474</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1161.1300000000001</v>
+      </c>
+      <c r="F21" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>2</v>
       </c>
       <c r="B22" s="1">
-        <v>0</v>
+        <v>16.459900000000001</v>
       </c>
       <c r="C22" s="1">
-        <v>60</v>
+        <v>10774.8</v>
       </c>
       <c r="D22" s="1">
-        <v>0</v>
+        <v>16.459900000000001</v>
       </c>
       <c r="E22" s="1">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>7870.87</v>
+      </c>
+      <c r="F22" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>3</v>
       </c>
       <c r="B23" s="2">
-        <v>0</v>
-      </c>
-      <c r="C23" s="1">
-        <v>60</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0</v>
-      </c>
-      <c r="E23" s="1">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>17.148</v>
+      </c>
+      <c r="C23" s="2">
+        <v>10554.7</v>
+      </c>
+      <c r="D23" s="1">
+        <v>17.148</v>
+      </c>
+      <c r="E23" s="2">
+        <v>6424.47</v>
+      </c>
+      <c r="F23" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>4</v>
       </c>
       <c r="B24" s="1">
-        <v>0</v>
+        <v>15.9971</v>
       </c>
       <c r="C24" s="1">
-        <v>65</v>
+        <v>10643.3</v>
       </c>
       <c r="D24" s="1">
-        <v>0</v>
+        <v>15.9971</v>
       </c>
       <c r="E24" s="1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>7769.39</v>
+      </c>
+      <c r="F24" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>5</v>
       </c>
       <c r="B25" s="1">
-        <v>0</v>
+        <v>16.123799999999999</v>
       </c>
       <c r="C25" s="1">
-        <v>57</v>
+        <v>10774.8</v>
       </c>
       <c r="D25" s="1">
-        <v>0</v>
-      </c>
-      <c r="E25" s="2">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>16.123799999999999</v>
+      </c>
+      <c r="E25" s="1">
+        <v>7160.13</v>
+      </c>
+      <c r="F25" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>6</v>
       </c>
       <c r="B26" s="1">
-        <v>0</v>
+        <v>16.096900000000002</v>
       </c>
       <c r="C26" s="1">
-        <v>76</v>
+        <v>10554.7</v>
       </c>
       <c r="D26" s="1">
-        <v>0</v>
+        <v>16.096900000000002</v>
       </c>
       <c r="E26" s="1">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>7788.77</v>
+      </c>
+      <c r="F26" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>7</v>
       </c>
       <c r="B27" s="1">
-        <v>0</v>
+        <v>16.0243</v>
       </c>
       <c r="C27" s="1">
-        <v>73</v>
+        <v>10554.7</v>
       </c>
       <c r="D27" s="1">
-        <v>0</v>
+        <v>16.0243</v>
       </c>
       <c r="E27" s="1">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>10554.7</v>
+      </c>
+      <c r="F27" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>8</v>
       </c>
       <c r="B28" s="2">
-        <v>0</v>
-      </c>
-      <c r="C28" s="1">
-        <v>86</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0</v>
-      </c>
-      <c r="E28" s="1">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>15.688800000000001</v>
+      </c>
+      <c r="C28" s="2">
+        <v>10554.7</v>
+      </c>
+      <c r="D28" s="1">
+        <v>15.688800000000001</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1995.16</v>
+      </c>
+      <c r="F28" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>9</v>
       </c>
       <c r="B29" s="1">
-        <v>0</v>
+        <v>16.334700000000002</v>
       </c>
       <c r="C29" s="1">
-        <v>79</v>
+        <v>10774.8</v>
       </c>
       <c r="D29" s="1">
-        <v>0</v>
+        <v>16.334700000000002</v>
       </c>
       <c r="E29" s="1">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>7856.72</v>
+      </c>
+      <c r="F29" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>10</v>
       </c>
       <c r="B30" s="2">
-        <v>0</v>
-      </c>
-      <c r="C30" s="1">
-        <v>89</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0</v>
-      </c>
-      <c r="E30" s="1">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>15.9864</v>
+      </c>
+      <c r="C30" s="2">
+        <v>10774.8</v>
+      </c>
+      <c r="D30" s="1">
+        <v>15.9864</v>
+      </c>
+      <c r="E30" s="2">
+        <v>544.51199999999994</v>
+      </c>
+      <c r="F30" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>11</v>
       </c>
       <c r="B31" s="2">
-        <v>0</v>
-      </c>
-      <c r="C31" s="1">
-        <v>61</v>
-      </c>
-      <c r="D31" s="2">
-        <v>1</v>
-      </c>
-      <c r="E31" s="1">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>16.615600000000001</v>
+      </c>
+      <c r="C31" s="2">
+        <v>10774.8</v>
+      </c>
+      <c r="D31" s="1">
+        <v>16.615600000000001</v>
+      </c>
+      <c r="E31" s="2">
+        <v>7788.77</v>
+      </c>
+      <c r="F31" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>12</v>
       </c>
       <c r="B32" s="1">
-        <v>0</v>
+        <v>15.9627</v>
       </c>
       <c r="C32" s="1">
-        <v>64</v>
+        <v>10774.8</v>
       </c>
       <c r="D32" s="1">
-        <v>0</v>
+        <v>15.9627</v>
       </c>
       <c r="E32" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>7300.28</v>
+      </c>
+      <c r="F32" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>13</v>
       </c>
       <c r="B33" s="2">
-        <v>0</v>
-      </c>
-      <c r="C33" s="1">
-        <v>89</v>
-      </c>
-      <c r="D33" s="2">
-        <v>0</v>
-      </c>
-      <c r="E33" s="1">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>16.154800000000002</v>
+      </c>
+      <c r="C33" s="2">
+        <v>10554.7</v>
+      </c>
+      <c r="D33" s="1">
+        <v>16.154800000000002</v>
+      </c>
+      <c r="E33" s="2">
+        <v>7788.77</v>
+      </c>
+      <c r="F33" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>14</v>
       </c>
       <c r="B34" s="1">
-        <v>0</v>
+        <v>16.110900000000001</v>
       </c>
       <c r="C34" s="1">
-        <v>67</v>
-      </c>
-      <c r="D34" s="2">
-        <v>0</v>
-      </c>
-      <c r="E34" s="1">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>10774.8</v>
+      </c>
+      <c r="D34" s="1">
+        <v>16.110900000000001</v>
+      </c>
+      <c r="E34" s="2">
+        <v>7788.77</v>
+      </c>
+      <c r="F34" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>15</v>
       </c>
       <c r="B35" s="1">
-        <v>0</v>
+        <v>15.9879</v>
       </c>
       <c r="C35" s="1">
-        <v>67</v>
+        <v>10774.9</v>
       </c>
       <c r="D35" s="1">
-        <v>0</v>
+        <v>15.9879</v>
       </c>
       <c r="E35" s="1">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>6623.12</v>
+      </c>
+      <c r="F35" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>16</v>
       </c>
       <c r="B36" s="1">
-        <v>0</v>
+        <v>15.9979</v>
       </c>
       <c r="C36" s="1">
-        <v>84</v>
+        <v>10554.7</v>
       </c>
       <c r="D36" s="1">
-        <v>0</v>
+        <v>15.9979</v>
       </c>
       <c r="E36" s="1">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>7209.11</v>
+      </c>
+      <c r="F36" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37">
         <v>17</v>
       </c>
       <c r="B37" s="1">
-        <v>0</v>
+        <v>16.367799999999999</v>
       </c>
       <c r="C37" s="1">
-        <v>57</v>
-      </c>
-      <c r="D37" s="2">
-        <v>0</v>
-      </c>
-      <c r="E37" s="1">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>10554.7</v>
+      </c>
+      <c r="D37" s="1">
+        <v>16.367799999999999</v>
+      </c>
+      <c r="E37" s="2">
+        <v>1705.71</v>
+      </c>
+      <c r="F37" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38">
         <v>18</v>
       </c>
       <c r="B38" s="2">
-        <v>0</v>
-      </c>
-      <c r="C38" s="1">
-        <v>62</v>
-      </c>
-      <c r="D38" s="2">
-        <v>1</v>
-      </c>
-      <c r="E38" s="1">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>15.668699999999999</v>
+      </c>
+      <c r="C38" s="2">
+        <v>10774.8</v>
+      </c>
+      <c r="D38" s="1">
+        <v>15.668699999999999</v>
+      </c>
+      <c r="E38" s="2">
+        <v>7856.72</v>
+      </c>
+      <c r="F38" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>19</v>
       </c>
       <c r="B39" s="2">
-        <v>0</v>
-      </c>
-      <c r="C39" s="1">
-        <v>64</v>
-      </c>
-      <c r="D39" s="2">
-        <v>1</v>
-      </c>
-      <c r="E39" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+        <v>16.698499999999999</v>
+      </c>
+      <c r="C39" s="2">
+        <v>10774.8</v>
+      </c>
+      <c r="D39" s="1">
+        <v>16.698499999999999</v>
+      </c>
+      <c r="E39" s="2">
+        <v>3131.76</v>
+      </c>
+      <c r="F39" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>20</v>
       </c>
       <c r="B40" s="2">
-        <v>0</v>
-      </c>
-      <c r="C40" s="1">
-        <v>58</v>
-      </c>
-      <c r="D40" s="2">
-        <v>0</v>
-      </c>
-      <c r="E40" s="1">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+        <v>16.6204</v>
+      </c>
+      <c r="C40" s="2">
+        <v>10570.8</v>
+      </c>
+      <c r="D40" s="1">
+        <v>16.6204</v>
+      </c>
+      <c r="E40" s="2">
+        <v>7505.06</v>
+      </c>
+      <c r="F40" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>21</v>
       </c>
       <c r="B41" s="1">
-        <v>0</v>
+        <v>16.0153</v>
       </c>
       <c r="C41" s="1">
-        <v>69</v>
+        <v>10774.8</v>
       </c>
       <c r="D41" s="1">
-        <v>0</v>
+        <v>16.0153</v>
       </c>
       <c r="E41" s="1">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+        <v>7788.77</v>
+      </c>
+      <c r="F41" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42">
         <v>22</v>
       </c>
       <c r="B42" s="1">
-        <v>0</v>
+        <v>16.3399</v>
       </c>
       <c r="C42" s="1">
-        <v>65</v>
+        <v>10554.7</v>
       </c>
       <c r="D42" s="1">
-        <v>0</v>
+        <v>16.3399</v>
       </c>
       <c r="E42" s="1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+        <v>366.01</v>
+      </c>
+      <c r="F42" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43">
         <v>23</v>
       </c>
       <c r="B43" s="2">
-        <v>0</v>
-      </c>
-      <c r="C43" s="1">
-        <v>47</v>
-      </c>
-      <c r="D43" s="2">
-        <v>0</v>
-      </c>
-      <c r="E43" s="1">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+        <v>16.1508</v>
+      </c>
+      <c r="C43" s="2">
+        <v>10554.7</v>
+      </c>
+      <c r="D43" s="1">
+        <v>16.1508</v>
+      </c>
+      <c r="E43" s="2">
+        <v>7505.06</v>
+      </c>
+      <c r="F43" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44">
         <v>24</v>
       </c>
       <c r="B44" s="1">
-        <v>0</v>
+        <v>16.024799999999999</v>
       </c>
       <c r="C44" s="1">
-        <v>66</v>
+        <v>10600.3</v>
       </c>
       <c r="D44" s="1">
-        <v>0</v>
+        <v>16.024799999999999</v>
       </c>
       <c r="E44" s="1">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+        <v>10554.7</v>
+      </c>
+      <c r="F44" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45">
         <v>25</v>
       </c>
       <c r="B45" s="2">
-        <v>0</v>
-      </c>
-      <c r="C45" s="1">
-        <v>65</v>
-      </c>
-      <c r="D45" s="2">
-        <v>0</v>
-      </c>
-      <c r="E45" s="1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>16.240100000000002</v>
+      </c>
+      <c r="C45" s="2">
+        <v>10554.7</v>
+      </c>
+      <c r="D45" s="1">
+        <v>16.240100000000002</v>
+      </c>
+      <c r="E45" s="2">
+        <v>1355.02</v>
+      </c>
+      <c r="F45" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46">
         <v>26</v>
       </c>
       <c r="B46" s="2">
-        <v>0</v>
-      </c>
-      <c r="C46" s="1">
-        <v>61</v>
-      </c>
-      <c r="D46" s="2">
-        <v>0</v>
-      </c>
-      <c r="E46" s="1">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+        <v>16.0044</v>
+      </c>
+      <c r="C46" s="2">
+        <v>10554.7</v>
+      </c>
+      <c r="D46" s="1">
+        <v>16.0044</v>
+      </c>
+      <c r="E46" s="2">
+        <v>7505.06</v>
+      </c>
+      <c r="F46" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47">
         <v>27</v>
       </c>
       <c r="B47" s="1">
-        <v>0</v>
+        <v>15.6934</v>
       </c>
       <c r="C47" s="1">
-        <v>63</v>
+        <v>10554.7</v>
       </c>
       <c r="D47" s="1">
-        <v>0</v>
+        <v>15.6934</v>
       </c>
       <c r="E47" s="1">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+        <v>1988.67</v>
+      </c>
+      <c r="F47" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48">
         <v>28</v>
       </c>
       <c r="B48" s="1">
-        <v>0</v>
+        <v>15.9495</v>
       </c>
       <c r="C48" s="1">
-        <v>61</v>
+        <v>10774.8</v>
       </c>
       <c r="D48" s="1">
-        <v>1</v>
+        <v>15.9495</v>
       </c>
       <c r="E48" s="1">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+        <v>237.215</v>
+      </c>
+      <c r="F48" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49">
         <v>29</v>
       </c>
       <c r="B49" s="1">
-        <v>0</v>
+        <v>15.956200000000001</v>
       </c>
       <c r="C49" s="1">
-        <v>63</v>
+        <v>10554.7</v>
       </c>
       <c r="D49" s="1">
-        <v>0</v>
+        <v>15.956200000000001</v>
       </c>
       <c r="E49" s="1">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+        <v>3161.81</v>
+      </c>
+      <c r="F49" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50">
         <v>30</v>
       </c>
       <c r="B50" s="1">
-        <v>0</v>
+        <v>16.1752</v>
       </c>
       <c r="C50" s="1">
-        <v>77</v>
+        <v>10774.8</v>
       </c>
       <c r="D50" s="1">
-        <v>0</v>
+        <v>16.1752</v>
       </c>
       <c r="E50" s="1">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+        <v>7169.58</v>
+      </c>
+      <c r="F50" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="3"/>
       <c r="B51" s="3">
         <f>AVERAGE(B21:B50)</f>
-        <v>0</v>
-      </c>
-      <c r="C51" s="4">
-        <f>AVERAGE(C21:C50)</f>
-        <v>68</v>
-      </c>
-      <c r="D51" s="3">
+        <v>16.171403333333338</v>
+      </c>
+      <c r="C51" s="3"/>
+      <c r="D51" s="4">
         <f>AVERAGE(D21:D50)</f>
-        <v>0.13333333333333333</v>
-      </c>
-      <c r="E51" s="3"/>
+        <v>16.171403333333338</v>
+      </c>
+      <c r="E51" s="3">
+        <f>AVERAGE(E21:E50)</f>
+        <v>5715.1939000000002</v>
+      </c>
+      <c r="F51" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated latex and xls.
</commit_message>
<xml_diff>
--- a/excel/Tablica.xlsx
+++ b/excel/Tablica.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="30260" yWindow="-3100" windowWidth="27320" windowHeight="13500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="13580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="30">
   <si>
     <t>simple</t>
   </si>
@@ -103,13 +103,19 @@
   </si>
   <si>
     <t>iprojekt</t>
+  </si>
+  <si>
+    <t>fitness</t>
+  </si>
+  <si>
+    <t>rank</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -160,8 +166,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,8 +241,19 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -231,8 +276,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
@@ -255,23 +328,66 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="11" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="17" applyFill="1"/>
-    <xf numFmtId="11" fontId="6" fillId="8" borderId="0" xfId="17" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="23" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="17" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="6" fillId="8" borderId="2" xfId="17" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="22" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="26"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="53">
+    <cellStyle name="Bad" xfId="22" builtinId="27"/>
     <cellStyle name="Explanatory Text" xfId="17" builtinId="53"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -282,6 +398,20 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -292,8 +422,24 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Neutral" xfId="26" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="2" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="23" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -622,398 +768,538 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:X51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="G5" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="8" max="8" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.625" customWidth="1"/>
+    <col min="19" max="19" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="9" t="s">
+      <c r="C1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="12" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" t="s">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D3">
+      <c r="B3" s="11">
+        <v>110.7628</v>
+      </c>
+      <c r="C3" s="11">
+        <v>1.1556010000000001</v>
+      </c>
+      <c r="D3" s="11">
         <v>3.9</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="11">
         <v>427.33333299999998</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="11">
         <v>1.1640448000000001</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="11">
         <v>0.63482333000000002</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="13">
         <v>5.8471999999999996E-16</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="14">
         <v>2.4171406700000002</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="14">
         <v>0</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="11">
         <v>30.747219999999999</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="14">
         <v>70.3</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="11">
         <v>16.364896699999999</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" t="s">
+      <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="B4" s="11">
+        <v>110.16325000000001</v>
+      </c>
+      <c r="C4" s="11">
+        <v>1.1233465</v>
+      </c>
+      <c r="D4" s="11">
         <v>5.3666660000000004</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="11">
         <v>486.96666670000002</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="11">
         <v>1.51229653</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="11">
         <v>6.4212023299999998</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="13">
         <v>7.2535000000000004E-16</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="11">
         <v>5.0484646700000004</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="11">
         <v>0.45233553999999998</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="11">
         <v>85.108540000000005</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="11">
         <v>59.4</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="11">
         <v>16.288783299999999</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" t="s">
+      <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
-        <v>111</v>
-      </c>
-      <c r="D5">
+      <c r="B5" s="11">
+        <v>110.36454999999999</v>
+      </c>
+      <c r="C5" s="11">
+        <v>1.1359809999999999</v>
+      </c>
+      <c r="D5" s="11">
         <v>4.8333329999999997</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="11">
         <v>461.7</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="11">
         <v>1.24346859</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="11">
         <v>3.9196123300000001</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="15">
         <v>7.5125000000000003E-16</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="11">
         <v>4.1872176699999999</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="11">
         <v>0.4976853</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="11">
         <v>62.800496699999997</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="13">
         <v>61.8</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="11">
         <v>16.171403300000001</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" t="s">
+      <c r="A6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D6">
+      <c r="B6" s="11">
+        <v>110.5621</v>
+      </c>
+      <c r="C6" s="11">
+        <v>1.1428195000000001</v>
+      </c>
+      <c r="D6" s="11">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="11">
         <v>431.76666667000001</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="11">
         <v>1.2003219300000001</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="11">
         <v>2.0041653300000002</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="13">
         <v>6.9204E-16</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="11">
         <v>4.6585486700000001</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="11">
         <v>0.18735260000000001</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="11">
         <v>27.226749300000002</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="11">
         <v>66.400000000000006</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="11">
         <v>16.221446700000001</v>
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" t="s">
+      <c r="A7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D7">
+      <c r="B7" s="11">
+        <v>109.66655</v>
+      </c>
+      <c r="C7" s="11">
+        <v>1.1313985</v>
+      </c>
+      <c r="D7" s="11">
         <v>4.2</v>
       </c>
-      <c r="F7">
+      <c r="E7" s="11">
+        <v>459.4</v>
+      </c>
+      <c r="F7" s="11">
         <v>1.6424551000000001</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="11">
         <v>5.2279523299999999</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="13">
         <v>9.835E-4</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="11">
         <v>6.5434099999999997</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="11">
         <v>0.82343434000000004</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="11">
         <v>51.458713299999999</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="11">
         <v>61.4</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="11">
         <v>16.312249999999999</v>
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" t="s">
+      <c r="A8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D8">
+      <c r="B8" s="11">
+        <v>110.76224999999999</v>
+      </c>
+      <c r="C8" s="11">
+        <v>1.1318275</v>
+      </c>
+      <c r="D8" s="11">
         <v>4.3</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="11">
         <v>476.53333300000003</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="11">
         <v>1.6177794700000001</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="11">
         <v>3.8770926700000001</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="13">
         <v>6.5872999999999996E-16</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="11">
         <v>5.1089936700000003</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="11">
         <v>0.13171603000000001</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="11">
         <v>59.151755000000001</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="11">
         <v>62.4</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="11">
         <v>16.222923300000001</v>
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" t="s">
+      <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11">
-        <v>0.26666659999999998</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="F9">
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="11">
         <v>2.0514364700000001</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="11">
         <v>3.8771770000000001</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="11">
         <v>5.0608299999999997E-3</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="11">
         <v>5.0862743300000002</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="11">
         <v>0.16171174999999999</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="11">
         <v>46.658380000000001</v>
       </c>
-      <c r="L9" s="12">
-        <v>58.8</v>
-      </c>
-      <c r="M9" s="11"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="18"/>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" t="s">
+      <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11">
-        <v>12.3</v>
-      </c>
-      <c r="E10" s="11"/>
-      <c r="F10">
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="11">
         <v>18.969425699999999</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="11">
         <v>10.622653</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="11">
         <v>2.1152359999999999</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="11">
         <v>12.636146699999999</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="11">
         <v>6.6285039299999999</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="11">
         <v>1078.7464299999999</v>
       </c>
-      <c r="L10" s="11">
-        <v>31.4</v>
-      </c>
-      <c r="M10" s="11"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="18"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" t="s">
+      <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D11">
+      <c r="B11" s="11">
+        <v>113.03155</v>
+      </c>
+      <c r="C11" s="11">
+        <v>1.1785794999999999</v>
+      </c>
+      <c r="D11" s="11">
         <v>13.966666</v>
       </c>
-      <c r="F11" s="8">
+      <c r="E11" s="11">
+        <v>727.13333299999999</v>
+      </c>
+      <c r="F11" s="19">
         <v>0.15859317000000001</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="14">
         <v>0.35</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="11">
         <v>0.43794266999999998</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="11">
         <v>3.0113536700000001</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="11">
         <v>0.13773753</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11" s="14">
         <v>15.9178143</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="11">
         <v>68</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="M11" s="11">
+        <v>16.152439999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24">
+      <c r="M17" s="20"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="20"/>
+    </row>
+    <row r="18" spans="1:24">
+      <c r="L18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N18" s="7"/>
+      <c r="O18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="P18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q18" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="R18" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="S18" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="T18" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="U18" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="V18" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="W18" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="X18" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24">
+      <c r="L19" s="11"/>
+      <c r="M19" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="N19" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="O19" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="P19" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q19" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="R19" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="S19" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="T19" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="U19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="V19" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="W19" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="X19" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1032,13 +1318,52 @@
       <c r="F20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="L20" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M20" s="21">
+        <v>2</v>
+      </c>
+      <c r="N20" s="11">
+        <v>2</v>
+      </c>
+      <c r="O20" s="14">
+        <v>1</v>
+      </c>
+      <c r="P20" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="11">
+        <v>2</v>
+      </c>
+      <c r="R20" s="11">
+        <v>2</v>
+      </c>
+      <c r="S20" s="13">
+        <v>4</v>
+      </c>
+      <c r="T20" s="14">
+        <v>1</v>
+      </c>
+      <c r="U20" s="14">
+        <v>1</v>
+      </c>
+      <c r="V20" s="11">
+        <v>3</v>
+      </c>
+      <c r="W20" s="3">
+        <v>1</v>
+      </c>
+      <c r="X20" s="11">
+        <v>16.364896699999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24">
       <c r="A21">
         <v>1</v>
       </c>
-      <c r="B21" s="1">
-        <v>16.5474</v>
+      <c r="B21">
+        <v>256</v>
       </c>
       <c r="C21" s="1">
         <v>10774.9</v>
@@ -1052,13 +1377,55 @@
       <c r="F21" s="2">
         <v>44</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="I21">
+        <v>111.06399999999999</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M21" s="22">
+        <v>6</v>
+      </c>
+      <c r="N21" s="11">
+        <v>7</v>
+      </c>
+      <c r="O21" s="11">
+        <v>6</v>
+      </c>
+      <c r="P21" s="11">
+        <v>6</v>
+      </c>
+      <c r="Q21" s="11">
+        <v>5</v>
+      </c>
+      <c r="R21" s="11">
+        <v>8</v>
+      </c>
+      <c r="S21" s="13">
+        <v>2</v>
+      </c>
+      <c r="T21" s="11">
+        <v>5</v>
+      </c>
+      <c r="U21" s="11">
+        <v>6</v>
+      </c>
+      <c r="V21" s="11">
+        <v>8</v>
+      </c>
+      <c r="W21" s="11">
+        <v>7</v>
+      </c>
+      <c r="X21" s="11">
+        <v>16.288783299999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24">
       <c r="A22">
         <v>2</v>
       </c>
-      <c r="B22" s="1">
-        <v>16.459900000000001</v>
+      <c r="B22">
+        <v>288</v>
       </c>
       <c r="C22" s="1">
         <v>10774.8</v>
@@ -1072,13 +1439,55 @@
       <c r="F22" s="1">
         <v>45</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="I22">
+        <v>109.072</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M22" s="22">
+        <v>5</v>
+      </c>
+      <c r="N22" s="11">
+        <v>5</v>
+      </c>
+      <c r="O22" s="11">
+        <v>5</v>
+      </c>
+      <c r="P22" s="11">
+        <v>4</v>
+      </c>
+      <c r="Q22" s="11">
+        <v>4</v>
+      </c>
+      <c r="R22" s="11">
+        <v>6</v>
+      </c>
+      <c r="S22" s="15">
+        <v>1</v>
+      </c>
+      <c r="T22" s="11">
+        <v>3</v>
+      </c>
+      <c r="U22" s="11">
+        <v>7</v>
+      </c>
+      <c r="V22" s="11">
+        <v>7</v>
+      </c>
+      <c r="W22" s="13">
+        <v>5</v>
+      </c>
+      <c r="X22" s="11">
+        <v>16.171403300000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24">
       <c r="A23">
         <v>3</v>
       </c>
-      <c r="B23" s="2">
-        <v>17.148</v>
+      <c r="B23">
+        <v>480</v>
       </c>
       <c r="C23" s="2">
         <v>10554.7</v>
@@ -1092,13 +1501,55 @@
       <c r="F23" s="1">
         <v>44</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="I23">
+        <v>111.062</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M23" s="22">
+        <v>4</v>
+      </c>
+      <c r="N23" s="11">
+        <v>3</v>
+      </c>
+      <c r="O23" s="11">
+        <v>4</v>
+      </c>
+      <c r="P23" s="11">
+        <v>2</v>
+      </c>
+      <c r="Q23" s="11">
+        <v>3</v>
+      </c>
+      <c r="R23" s="11">
+        <v>3</v>
+      </c>
+      <c r="S23" s="13">
+        <v>5</v>
+      </c>
+      <c r="T23" s="11">
+        <v>4</v>
+      </c>
+      <c r="U23" s="11">
+        <v>5</v>
+      </c>
+      <c r="V23" s="11">
+        <v>2</v>
+      </c>
+      <c r="W23" s="11">
+        <v>3</v>
+      </c>
+      <c r="X23" s="11">
+        <v>16.221446700000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24">
       <c r="A24">
         <v>4</v>
       </c>
-      <c r="B24" s="1">
-        <v>15.9971</v>
+      <c r="B24">
+        <v>492</v>
       </c>
       <c r="C24" s="1">
         <v>10643.3</v>
@@ -1112,13 +1563,55 @@
       <c r="F24" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="I24">
+        <v>111.06100000000001</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M24" s="22">
+        <v>7</v>
+      </c>
+      <c r="N24" s="11">
+        <v>6</v>
+      </c>
+      <c r="O24" s="11">
+        <v>2</v>
+      </c>
+      <c r="P24" s="11">
+        <v>3</v>
+      </c>
+      <c r="Q24" s="11">
+        <v>7</v>
+      </c>
+      <c r="R24" s="11">
+        <v>7</v>
+      </c>
+      <c r="S24" s="13">
+        <v>6</v>
+      </c>
+      <c r="T24" s="11">
+        <v>8</v>
+      </c>
+      <c r="U24" s="11">
+        <v>8</v>
+      </c>
+      <c r="V24" s="11">
+        <v>5</v>
+      </c>
+      <c r="W24" s="11">
+        <v>6</v>
+      </c>
+      <c r="X24" s="11">
+        <v>16.312249999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24">
       <c r="A25">
         <v>5</v>
       </c>
-      <c r="B25" s="1">
-        <v>16.123799999999999</v>
+      <c r="B25">
+        <v>504</v>
       </c>
       <c r="C25" s="1">
         <v>10774.8</v>
@@ -1132,13 +1625,55 @@
       <c r="F25" s="2">
         <v>42</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="I25">
+        <v>111.065</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M25" s="22">
+        <v>3</v>
+      </c>
+      <c r="N25" s="11">
+        <v>4</v>
+      </c>
+      <c r="O25" s="11">
+        <v>3</v>
+      </c>
+      <c r="P25" s="11">
+        <v>5</v>
+      </c>
+      <c r="Q25" s="11">
+        <v>6</v>
+      </c>
+      <c r="R25" s="11">
+        <v>4</v>
+      </c>
+      <c r="S25" s="13">
+        <v>3</v>
+      </c>
+      <c r="T25" s="11">
+        <v>7</v>
+      </c>
+      <c r="U25" s="11">
+        <v>2</v>
+      </c>
+      <c r="V25" s="11">
+        <v>6</v>
+      </c>
+      <c r="W25" s="11">
+        <v>4</v>
+      </c>
+      <c r="X25" s="11">
+        <v>16.222923300000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24">
       <c r="A26">
         <v>6</v>
       </c>
-      <c r="B26" s="1">
-        <v>16.096900000000002</v>
+      <c r="B26">
+        <v>524</v>
       </c>
       <c r="C26" s="1">
         <v>10554.7</v>
@@ -1152,13 +1687,43 @@
       <c r="F26" s="1">
         <v>46</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="I26">
+        <v>111.06100000000001</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M26" s="23"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="11">
+        <v>8</v>
+      </c>
+      <c r="R26" s="11">
+        <v>5</v>
+      </c>
+      <c r="S26" s="11">
+        <v>7</v>
+      </c>
+      <c r="T26" s="11">
+        <v>6</v>
+      </c>
+      <c r="U26" s="11">
+        <v>4</v>
+      </c>
+      <c r="V26" s="11">
+        <v>4</v>
+      </c>
+      <c r="W26" s="17"/>
+      <c r="X26" s="18"/>
+    </row>
+    <row r="27" spans="1:24">
       <c r="A27">
         <v>7</v>
       </c>
-      <c r="B27" s="1">
-        <v>16.0243</v>
+      <c r="B27">
+        <v>476</v>
       </c>
       <c r="C27" s="1">
         <v>10554.7</v>
@@ -1172,13 +1737,43 @@
       <c r="F27" s="1">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="I27">
+        <v>111.06100000000001</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M27" s="23"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="11">
+        <v>9</v>
+      </c>
+      <c r="R27" s="11">
+        <v>9</v>
+      </c>
+      <c r="S27" s="11">
+        <v>9</v>
+      </c>
+      <c r="T27" s="11">
+        <v>9</v>
+      </c>
+      <c r="U27" s="11">
+        <v>9</v>
+      </c>
+      <c r="V27" s="11">
+        <v>9</v>
+      </c>
+      <c r="W27" s="16"/>
+      <c r="X27" s="18"/>
+    </row>
+    <row r="28" spans="1:24">
       <c r="A28">
         <v>8</v>
       </c>
-      <c r="B28" s="2">
-        <v>15.688800000000001</v>
+      <c r="B28">
+        <v>396</v>
       </c>
       <c r="C28" s="2">
         <v>10554.7</v>
@@ -1192,13 +1787,55 @@
       <c r="F28" s="1">
         <v>44</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="I28">
+        <v>111.06399999999999</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M28" s="22">
+        <v>1</v>
+      </c>
+      <c r="N28" s="14">
+        <v>1</v>
+      </c>
+      <c r="O28" s="11">
+        <v>7</v>
+      </c>
+      <c r="P28" s="11">
+        <v>7</v>
+      </c>
+      <c r="Q28" s="14">
+        <v>1</v>
+      </c>
+      <c r="R28" s="14">
+        <v>1</v>
+      </c>
+      <c r="S28" s="11">
+        <v>8</v>
+      </c>
+      <c r="T28" s="11">
+        <v>2</v>
+      </c>
+      <c r="U28" s="11">
+        <v>3</v>
+      </c>
+      <c r="V28" s="14">
+        <v>1</v>
+      </c>
+      <c r="W28" s="11">
+        <v>2</v>
+      </c>
+      <c r="X28" s="11">
+        <v>16.152439999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24">
       <c r="A29">
         <v>9</v>
       </c>
-      <c r="B29" s="1">
-        <v>16.334700000000002</v>
+      <c r="B29">
+        <v>544</v>
       </c>
       <c r="C29" s="1">
         <v>10774.8</v>
@@ -1212,13 +1849,16 @@
       <c r="F29" s="1">
         <v>46</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="I29">
+        <v>111.066</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24">
       <c r="A30">
         <v>10</v>
       </c>
-      <c r="B30" s="2">
-        <v>15.9864</v>
+      <c r="B30">
+        <v>440</v>
       </c>
       <c r="C30" s="2">
         <v>10774.8</v>
@@ -1232,13 +1872,16 @@
       <c r="F30" s="1">
         <v>42</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="I30">
+        <v>111.063</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24">
       <c r="A31">
         <v>11</v>
       </c>
-      <c r="B31" s="2">
-        <v>16.615600000000001</v>
+      <c r="B31">
+        <v>416</v>
       </c>
       <c r="C31" s="2">
         <v>10774.8</v>
@@ -1252,13 +1895,16 @@
       <c r="F31" s="1">
         <v>44</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="I31">
+        <v>109.071</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24">
       <c r="A32">
         <v>12</v>
       </c>
-      <c r="B32" s="1">
-        <v>15.9627</v>
+      <c r="B32">
+        <v>528</v>
       </c>
       <c r="C32" s="1">
         <v>10774.8</v>
@@ -1272,13 +1918,16 @@
       <c r="F32" s="1">
         <v>42</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="I32">
+        <v>111.066</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33">
         <v>13</v>
       </c>
-      <c r="B33" s="2">
-        <v>16.154800000000002</v>
+      <c r="B33">
+        <v>464</v>
       </c>
       <c r="C33" s="2">
         <v>10554.7</v>
@@ -1292,13 +1941,16 @@
       <c r="F33" s="1">
         <v>44</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="I33">
+        <v>111.062</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34">
         <v>14</v>
       </c>
-      <c r="B34" s="1">
-        <v>16.110900000000001</v>
+      <c r="B34">
+        <v>448</v>
       </c>
       <c r="C34" s="1">
         <v>10774.8</v>
@@ -1312,13 +1964,16 @@
       <c r="F34" s="1">
         <v>46</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="I34">
+        <v>109.07</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35">
         <v>15</v>
       </c>
-      <c r="B35" s="1">
-        <v>15.9879</v>
+      <c r="B35">
+        <v>400</v>
       </c>
       <c r="C35" s="1">
         <v>10774.9</v>
@@ -1332,13 +1987,16 @@
       <c r="F35" s="1">
         <v>43</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="I35">
+        <v>111.059</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36">
         <v>16</v>
       </c>
-      <c r="B36" s="1">
-        <v>15.9979</v>
+      <c r="B36">
+        <v>464</v>
       </c>
       <c r="C36" s="1">
         <v>10554.7</v>
@@ -1352,13 +2010,16 @@
       <c r="F36" s="1">
         <v>46</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="I36">
+        <v>109.07</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37">
         <v>17</v>
       </c>
-      <c r="B37" s="1">
-        <v>16.367799999999999</v>
+      <c r="B37">
+        <v>640</v>
       </c>
       <c r="C37" s="1">
         <v>10554.7</v>
@@ -1372,13 +2033,16 @@
       <c r="F37" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="I37">
+        <v>111.065</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38">
         <v>18</v>
       </c>
-      <c r="B38" s="2">
-        <v>15.668699999999999</v>
+      <c r="B38">
+        <v>528</v>
       </c>
       <c r="C38" s="2">
         <v>10774.8</v>
@@ -1392,13 +2056,16 @@
       <c r="F38" s="1">
         <v>44</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="I38">
+        <v>111.059</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39">
         <v>19</v>
       </c>
-      <c r="B39" s="2">
-        <v>16.698499999999999</v>
+      <c r="B39">
+        <v>352</v>
       </c>
       <c r="C39" s="2">
         <v>10774.8</v>
@@ -1412,13 +2079,16 @@
       <c r="F39" s="1">
         <v>44</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="I39">
+        <v>113.02</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40">
         <v>20</v>
       </c>
-      <c r="B40" s="2">
-        <v>16.6204</v>
+      <c r="B40">
+        <v>288</v>
       </c>
       <c r="C40" s="2">
         <v>10570.8</v>
@@ -1432,13 +2102,16 @@
       <c r="F40" s="1">
         <v>43</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="I40">
+        <v>111.06399999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41">
         <v>21</v>
       </c>
-      <c r="B41" s="1">
-        <v>16.0153</v>
+      <c r="B41">
+        <v>672</v>
       </c>
       <c r="C41" s="1">
         <v>10774.8</v>
@@ -1452,13 +2125,17 @@
       <c r="F41" s="1">
         <v>42</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="I41" s="3">
+        <f>AVERAGE(I21:I40)</f>
+        <v>110.76224999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42">
         <v>22</v>
       </c>
-      <c r="B42" s="1">
-        <v>16.3399</v>
+      <c r="B42">
+        <v>416</v>
       </c>
       <c r="C42" s="1">
         <v>10554.7</v>
@@ -1473,12 +2150,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:9">
       <c r="A43">
         <v>23</v>
       </c>
-      <c r="B43" s="2">
-        <v>16.1508</v>
+      <c r="B43">
+        <v>392</v>
       </c>
       <c r="C43" s="2">
         <v>10554.7</v>
@@ -1493,12 +2170,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:9">
       <c r="A44">
         <v>24</v>
       </c>
-      <c r="B44" s="1">
-        <v>16.024799999999999</v>
+      <c r="B44">
+        <v>576</v>
       </c>
       <c r="C44" s="1">
         <v>10600.3</v>
@@ -1513,12 +2190,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:9">
       <c r="A45">
         <v>25</v>
       </c>
-      <c r="B45" s="2">
-        <v>16.240100000000002</v>
+      <c r="B45">
+        <v>520</v>
       </c>
       <c r="C45" s="2">
         <v>10554.7</v>
@@ -1533,12 +2210,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:9">
       <c r="A46">
         <v>26</v>
       </c>
-      <c r="B46" s="2">
-        <v>16.0044</v>
+      <c r="B46">
+        <v>336</v>
       </c>
       <c r="C46" s="2">
         <v>10554.7</v>
@@ -1553,12 +2230,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:9">
       <c r="A47">
         <v>27</v>
       </c>
-      <c r="B47" s="1">
-        <v>15.6934</v>
+      <c r="B47">
+        <v>628</v>
       </c>
       <c r="C47" s="1">
         <v>10554.7</v>
@@ -1573,12 +2250,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:9">
       <c r="A48">
         <v>28</v>
       </c>
-      <c r="B48" s="1">
-        <v>15.9495</v>
+      <c r="B48">
+        <v>488</v>
       </c>
       <c r="C48" s="1">
         <v>10774.8</v>
@@ -1597,8 +2274,8 @@
       <c r="A49">
         <v>29</v>
       </c>
-      <c r="B49" s="1">
-        <v>15.956200000000001</v>
+      <c r="B49">
+        <v>564</v>
       </c>
       <c r="C49" s="1">
         <v>10554.7</v>
@@ -1617,8 +2294,8 @@
       <c r="A50">
         <v>30</v>
       </c>
-      <c r="B50" s="1">
-        <v>16.1752</v>
+      <c r="B50">
+        <v>262</v>
       </c>
       <c r="C50" s="1">
         <v>10774.8</v>
@@ -1637,7 +2314,7 @@
       <c r="A51" s="3"/>
       <c r="B51" s="3">
         <f>AVERAGE(B21:B50)</f>
-        <v>16.171403333333338</v>
+        <v>459.4</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="4">

</xml_diff>